<commit_message>
Corrected 'bicubic' to 'cubic', updated sm.py to data reader
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\python-backend-data-visualization-matplotlib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\simple-install\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A4F4C4-CC99-4828-BBAB-8491452A8B93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6406DDA-440D-4B38-ADBC-E9DE899D8CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6A099C5A-765B-46B2-8CBE-4594BEE6E231}"/>
   </bookViews>
@@ -416,7 +416,7 @@
   <dimension ref="C1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>